<commit_message>
Modif Excel Cours 24/10
</commit_message>
<xml_diff>
--- a/doc/organisation/planning.xlsx
+++ b/doc/organisation/planning.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\castrignano.vincenzo\Documents\Cours\2e_annee\Github\BSN_2024\doc\organisation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beaudouin.eliott\AndroidStudioProjects\BSN_2024\doc\organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F32F3D-035F-4C27-961D-829A762C3A1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED040D4-A879-453D-B369-72B641E5C481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" xr2:uid="{C5453DEA-48C7-49DC-ABD6-6D9F04A40713}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8256" activeTab="1" xr2:uid="{C5453DEA-48C7-49DC-ABD6-6D9F04A40713}"/>
   </bookViews>
   <sheets>
     <sheet name="20oct" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
   <si>
     <t>Nicolas PATIGNY</t>
   </si>
@@ -109,6 +110,78 @@
   </si>
   <si>
     <t>Rien fait</t>
+  </si>
+  <si>
+    <t>Fait ?</t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>Liste tâches début cours 24/10</t>
+  </si>
+  <si>
+    <t>Apparemment ?</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>1h30</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>2h30</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>Git/ Tuto .md</t>
+  </si>
+  <si>
+    <t>Cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> moi</t>
+  </si>
+  <si>
+    <t>Karim/mika</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>manip kotlin</t>
+  </si>
+  <si>
+    <t>Cours/M</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Eliott</t>
+  </si>
+  <si>
+    <t>Alhouss</t>
+  </si>
+  <si>
+    <t>Proto</t>
   </si>
 </sst>
 </file>
@@ -292,36 +365,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
@@ -329,9 +372,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,6 +379,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -657,239 +730,394 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0B2124-A31E-4B24-9212-BB2D4AD7A846}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="8" width="35.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="8" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="14" t="s">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="D27" s="15" t="s">
+      <c r="B27" s="11"/>
+      <c r="D27" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="D28" s="16" t="s">
+      <c r="B28" s="14"/>
+      <c r="D28" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="D29" s="16" t="s">
+      <c r="B29" s="14"/>
+      <c r="D29" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="D30" s="17" t="s">
+      <c r="B30" s="14"/>
+      <c r="D30" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="B31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="B32" s="14"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="8"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="9" t="s">
+      <c r="B33" s="14"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="10"/>
+      <c r="B34" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="B1:H3"/>
     <mergeCell ref="A1:A3"/>
@@ -900,16 +1128,275 @@
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:H14"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:H5" xr:uid="{2CAB0C69-761D-438C-A335-BB958AD0587A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:H5 B16:H16" xr:uid="{2CAB0C69-761D-438C-A335-BB958AD0587A}">
       <formula1>$A$28:$A$34</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:H8" xr:uid="{60E06066-FB2E-4F77-A2BF-FD825F0AD299}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:H8 B19:H19" xr:uid="{60E06066-FB2E-4F77-A2BF-FD825F0AD299}">
       <formula1>$D$28:$D$30</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF737070-5679-4FB8-BB19-EAAD698E5383}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:H3"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:H8" xr:uid="{67F17534-4A33-44F5-9798-51A02AC03F74}">
+      <formula1>$D$28:$D$30</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:H5" xr:uid="{0D9645B5-96F9-4933-A1A7-968FB7706898}">
+      <formula1>$A$28:$A$34</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout Excel 24/10 modif
</commit_message>
<xml_diff>
--- a/doc/organisation/planning.xlsx
+++ b/doc/organisation/planning.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beaudouin.eliott\AndroidStudioProjects\BSN_2024\doc\organisation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\castrignano.vincenzo\Documents\Cours\2e_annee\Github\BSN_2024\doc\organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED040D4-A879-453D-B369-72B641E5C481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C5B4FA-E7AB-4F36-9C36-341223C1BD0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8256" activeTab="1" xr2:uid="{C5453DEA-48C7-49DC-ABD6-6D9F04A40713}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8260" activeTab="2" xr2:uid="{C5453DEA-48C7-49DC-ABD6-6D9F04A40713}"/>
   </bookViews>
   <sheets>
     <sheet name="20oct" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
+    <sheet name="24oct" sheetId="3" r:id="rId2"/>
+    <sheet name="26oct" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="46">
   <si>
     <t>Nicolas PATIGNY</t>
   </si>
@@ -148,40 +149,22 @@
     <t>4h</t>
   </si>
   <si>
-    <t>Git/ Tuto .md</t>
-  </si>
-  <si>
-    <t>Cours</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> moi</t>
-  </si>
-  <si>
-    <t>Karim/mika</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>manip kotlin</t>
-  </si>
-  <si>
-    <t>Cours/M</t>
-  </si>
-  <si>
-    <t>Nico</t>
-  </si>
-  <si>
-    <t>Eliott</t>
-  </si>
-  <si>
-    <t>Alhouss</t>
-  </si>
-  <si>
-    <t>Proto</t>
+    <t>Liste des répartitions des tâches 24/10</t>
+  </si>
+  <si>
+    <t>Liste tâches début cours 26/10</t>
+  </si>
+  <si>
+    <t>Tuto .md + Tackboard</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Liste des répartitions des tâches 26/10</t>
+  </si>
+  <si>
+    <t>Liste tâches début cours 18/11</t>
   </si>
 </sst>
 </file>
@@ -730,17 +713,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0B2124-A31E-4B24-9212-BB2D4AD7A846}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:H8"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="8" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="8" width="35.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="9" t="s">
         <v>11</v>
@@ -752,7 +735,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13"/>
@@ -762,7 +745,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15"/>
       <c r="B3" s="7"/>
       <c r="C3" s="15"/>
@@ -772,7 +755,7 @@
       <c r="G3" s="15"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -796,7 +779,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -822,7 +805,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -848,7 +831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -874,7 +857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -900,8 +883,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="9" t="s">
         <v>30</v>
@@ -913,7 +896,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -923,7 +906,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="15"/>
       <c r="B14" s="7"/>
       <c r="C14" s="15"/>
@@ -933,7 +916,7 @@
       <c r="G14" s="15"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>0</v>
@@ -957,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -983,7 +966,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1005,9 +988,11 @@
       <c r="G17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H17" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1029,9 +1014,11 @@
       <c r="G18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1053,10 +1040,12 @@
       <c r="G19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1054,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>13</v>
       </c>
@@ -1074,7 +1063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>14</v>
       </c>
@@ -1083,7 +1072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="12" t="s">
         <v>15</v>
       </c>
@@ -1092,25 +1081,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="14"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="14"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="14"/>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="7" t="s">
         <v>19</v>
       </c>
@@ -1145,19 +1134,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF737070-5679-4FB8-BB19-EAAD698E5383}">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459C1FE9-96DD-48BF-8242-16CC046FAB81}">
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="61" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="8" width="35.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1166,7 +1159,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13"/>
@@ -1176,7 +1169,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15"/>
       <c r="B3" s="7"/>
       <c r="C3" s="15"/>
@@ -1186,7 +1179,7 @@
       <c r="G3" s="15"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1210,7 +1203,374 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="16"/>
+      <c r="B12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="16"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="15"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="D27" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="D28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="D29" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="D30" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="14"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="14"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:H3"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:H14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:H8 B19:H19" xr:uid="{BA4D649F-476D-443F-B12E-A386483964C3}">
+      <formula1>$D$28:$D$30</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:H5 B16:H16" xr:uid="{355B3294-809B-4973-A2CF-605E122775E5}">
+      <formula1>$A$28:$A$34</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A969E59-ADB1-47B3-847A-9B6B120D6FB7}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="8" width="35.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="16"/>
+      <c r="B1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1222,179 +1582,229 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="16"/>
+      <c r="B12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="16"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="15"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="D27" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="D28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="D29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="3" t="s">
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="D30" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="14"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="14"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
+      <c r="B34" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="12">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:H3"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:H14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:H8" xr:uid="{67F17534-4A33-44F5-9798-51A02AC03F74}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:H5 B16:H16" xr:uid="{5D1E45F0-BE56-4238-BFF5-C2DE4C05493F}">
+      <formula1>$A$28:$A$34</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:H8 B19:H19" xr:uid="{EFA00A6E-AAEC-4803-BA92-CD95E0F5BE03}">
       <formula1>$D$28:$D$30</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:H5" xr:uid="{0D9645B5-96F9-4933-A1A7-968FB7706898}">
-      <formula1>$A$28:$A$34</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modif Readme / Ajout Equipe
</commit_message>
<xml_diff>
--- a/doc/organisation/planning.xlsx
+++ b/doc/organisation/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\castrignano.vincenzo\Documents\Cours\2e_annee\Github\BSN_2024\doc\organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C5B4FA-E7AB-4F36-9C36-341223C1BD0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AF612A-BE2E-4CC8-8487-CF54582FCF33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8260" activeTab="2" xr2:uid="{C5453DEA-48C7-49DC-ABD6-6D9F04A40713}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8260" xr2:uid="{C5453DEA-48C7-49DC-ABD6-6D9F04A40713}"/>
   </bookViews>
   <sheets>
     <sheet name="20oct" sheetId="1" r:id="rId1"/>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0B2124-A31E-4B24-9212-BB2D4AD7A846}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1504,7 +1504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A969E59-ADB1-47B3-847A-9B6B120D6FB7}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+    <sheetView zoomScale="57" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajout tuto Kotlin, partie variable, fonction Amélioration du md
</commit_message>
<xml_diff>
--- a/doc/organisation/planning.xlsx
+++ b/doc/organisation/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\castrignano.vincenzo\Documents\Cours\2e_annee\Github\BSN_2024\doc\organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5053DB72-F779-486E-BCFB-9680BC51333E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9816799E-627B-43C5-85C3-8FE6212F2E68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8260" activeTab="2" xr2:uid="{C5453DEA-48C7-49DC-ABD6-6D9F04A40713}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="50">
   <si>
     <t>Nicolas PATIGNY</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Taskboard + début prototype function</t>
+  </si>
+  <si>
+    <t>Groupe de tâches</t>
   </si>
 </sst>
 </file>
@@ -722,7 +725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0B2124-A31E-4B24-9212-BB2D4AD7A846}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
@@ -1567,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A969E59-ADB1-47B3-847A-9B6B120D6FB7}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1837,7 +1840,7 @@
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B27" s="11"/>
       <c r="D27" s="4" t="s">

</xml_diff>